<commit_message>
Add visualization to number of clients connected and average RAM usage
</commit_message>
<xml_diff>
--- a/live_resource_summary.xlsx
+++ b/live_resource_summary.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -743,6 +743,1070 @@
         <v>8526</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>m_UJXwLhTD1dkUskAAAB</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:19:36.284683</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>75.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K6" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L6" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M6" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2727.06</v>
+      </c>
+      <c r="O6" t="n">
+        <v>21930.86</v>
+      </c>
+      <c r="P6" t="n">
+        <v>422311</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>lYKrMQoRT92zl1UBAAAD</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:19:40.396581</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="I7" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K7" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L7" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M7" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2727.06</v>
+      </c>
+      <c r="O7" t="n">
+        <v>21930.86</v>
+      </c>
+      <c r="P7" t="n">
+        <v>422317</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IRd7AOBvHtV5FvyIAAAB</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:21:17.771054</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="I8" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="J8" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K8" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L8" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M8" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2727.14</v>
+      </c>
+      <c r="O8" t="n">
+        <v>21931.03</v>
+      </c>
+      <c r="P8" t="n">
+        <v>422414</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>6rF8v1ZrhbBS63UuAAAB</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:22:02.591642</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="I9" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K9" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L9" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M9" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2727.27</v>
+      </c>
+      <c r="O9" t="n">
+        <v>21932.67</v>
+      </c>
+      <c r="P9" t="n">
+        <v>422459</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TW3RIBjtp7MwyWOtAAAB</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:24:26.327092</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="I10" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="J10" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K10" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L10" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M10" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2727.56</v>
+      </c>
+      <c r="O10" t="n">
+        <v>21933.3</v>
+      </c>
+      <c r="P10" t="n">
+        <v>422602</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dt7blYupXMA6NAVIAAAF</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:24:42.286716</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="I11" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="J11" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K11" t="n">
+        <v>358.46</v>
+      </c>
+      <c r="L11" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="M11" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2727.57</v>
+      </c>
+      <c r="O11" t="n">
+        <v>21933.31</v>
+      </c>
+      <c r="P11" t="n">
+        <v>422618</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0KfCrwcFavwV9gfjAAAD</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-06-23T19:26:52.729032</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="I12" t="n">
+        <v>76.2</v>
+      </c>
+      <c r="J12" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K12" t="n">
+        <v>358.47</v>
+      </c>
+      <c r="L12" t="n">
+        <v>120.1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2727.83</v>
+      </c>
+      <c r="O12" t="n">
+        <v>21937.6</v>
+      </c>
+      <c r="P12" t="n">
+        <v>422748</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>H3NI-JvLota0t9C_AAAD</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:13:19.899369</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12</v>
+      </c>
+      <c r="G13" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="I13" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K13" t="n">
+        <v>354.84</v>
+      </c>
+      <c r="L13" t="n">
+        <v>123.72</v>
+      </c>
+      <c r="M13" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2732.71</v>
+      </c>
+      <c r="O13" t="n">
+        <v>21969.04</v>
+      </c>
+      <c r="P13" t="n">
+        <v>425536</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>FA1J7YAflWOz1GkOAAAB</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:13:36.306918</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="I14" t="n">
+        <v>75.59999999999999</v>
+      </c>
+      <c r="J14" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K14" t="n">
+        <v>354.84</v>
+      </c>
+      <c r="L14" t="n">
+        <v>123.72</v>
+      </c>
+      <c r="M14" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2732.73</v>
+      </c>
+      <c r="O14" t="n">
+        <v>21969.2</v>
+      </c>
+      <c r="P14" t="n">
+        <v>425552</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>fyCd0DbuhXS4jsTUAAAB</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:18:04.519644</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>12</v>
+      </c>
+      <c r="G15" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="I15" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="J15" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K15" t="n">
+        <v>354.85</v>
+      </c>
+      <c r="L15" t="n">
+        <v>123.72</v>
+      </c>
+      <c r="M15" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2733.28</v>
+      </c>
+      <c r="O15" t="n">
+        <v>21979.41</v>
+      </c>
+      <c r="P15" t="n">
+        <v>425820</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>lNpVG2frpMuTZVhiAAAB</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:22:39.440671</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6</v>
+      </c>
+      <c r="F16" t="n">
+        <v>12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="I16" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="J16" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K16" t="n">
+        <v>355.51</v>
+      </c>
+      <c r="L16" t="n">
+        <v>123.05</v>
+      </c>
+      <c r="M16" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2736.33</v>
+      </c>
+      <c r="O16" t="n">
+        <v>22057.7</v>
+      </c>
+      <c r="P16" t="n">
+        <v>426095</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>I5kSiq3vZPgkd909AAAD</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:22:11.425098</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="I17" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="J17" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K17" t="n">
+        <v>354.85</v>
+      </c>
+      <c r="L17" t="n">
+        <v>123.72</v>
+      </c>
+      <c r="M17" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2733.63</v>
+      </c>
+      <c r="O17" t="n">
+        <v>21980.19</v>
+      </c>
+      <c r="P17" t="n">
+        <v>426068</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>i1EQthTdsICGr0tPAAAB</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:30:00.963646</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="I18" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="J18" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K18" t="n">
+        <v>355.97</v>
+      </c>
+      <c r="L18" t="n">
+        <v>122.6</v>
+      </c>
+      <c r="M18" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2742.4</v>
+      </c>
+      <c r="O18" t="n">
+        <v>22244.01</v>
+      </c>
+      <c r="P18" t="n">
+        <v>426537</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>wmcC2IxsVpeVnlihAAAD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:30:51.282474</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="I19" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="J19" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K19" t="n">
+        <v>355.98</v>
+      </c>
+      <c r="L19" t="n">
+        <v>122.59</v>
+      </c>
+      <c r="M19" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2742.49</v>
+      </c>
+      <c r="O19" t="n">
+        <v>22244.27</v>
+      </c>
+      <c r="P19" t="n">
+        <v>426586</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ZuagEM0cT0mcrRl2AAAB</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:32:56.151638</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>12</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="I20" t="n">
+        <v>85</v>
+      </c>
+      <c r="J20" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K20" t="n">
+        <v>355.98</v>
+      </c>
+      <c r="L20" t="n">
+        <v>122.58</v>
+      </c>
+      <c r="M20" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2742.97</v>
+      </c>
+      <c r="O20" t="n">
+        <v>22249.57</v>
+      </c>
+      <c r="P20" t="n">
+        <v>426712</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Qg5WSfydU5N9Bo4ZAAAB</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:35:58.509543</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>12</v>
+      </c>
+      <c r="G21" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="I21" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="J21" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K21" t="n">
+        <v>355.99</v>
+      </c>
+      <c r="L21" t="n">
+        <v>122.58</v>
+      </c>
+      <c r="M21" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2743.35</v>
+      </c>
+      <c r="O21" t="n">
+        <v>22250.3</v>
+      </c>
+      <c r="P21" t="n">
+        <v>426894</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>h9VAKK8hhR_n6VT-AAAH</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:36:31.457148</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" t="n">
+        <v>12</v>
+      </c>
+      <c r="G22" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="I22" t="n">
+        <v>89.3</v>
+      </c>
+      <c r="J22" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K22" t="n">
+        <v>356</v>
+      </c>
+      <c r="L22" t="n">
+        <v>122.57</v>
+      </c>
+      <c r="M22" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N22" t="n">
+        <v>2743.71</v>
+      </c>
+      <c r="O22" t="n">
+        <v>22253.74</v>
+      </c>
+      <c r="P22" t="n">
+        <v>426927</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BcxAwbh-lJeGmq9VAAAB</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:40:37.525796</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12</v>
+      </c>
+      <c r="G23" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="I23" t="n">
+        <v>88.40000000000001</v>
+      </c>
+      <c r="J23" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K23" t="n">
+        <v>356.02</v>
+      </c>
+      <c r="L23" t="n">
+        <v>122.55</v>
+      </c>
+      <c r="M23" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2744.64</v>
+      </c>
+      <c r="O23" t="n">
+        <v>22260.78</v>
+      </c>
+      <c r="P23" t="n">
+        <v>427174</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>xsN27XdOX2Dy7tHGAAAB</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-06-23T20:44:08.952665</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Windows-11-10.0.26100-SP0</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="I24" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="J24" t="n">
+        <v>478.57</v>
+      </c>
+      <c r="K24" t="n">
+        <v>356.02</v>
+      </c>
+      <c r="L24" t="n">
+        <v>122.55</v>
+      </c>
+      <c r="M24" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="N24" t="n">
+        <v>2745.45</v>
+      </c>
+      <c r="O24" t="n">
+        <v>22274.42</v>
+      </c>
+      <c r="P24" t="n">
+        <v>427384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>